<commit_message>
update project structure and deployment files
</commit_message>
<xml_diff>
--- a/web/data/label.xlsx
+++ b/web/data/label.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8903dcf0377865c7/Dokumen/Punya Zahran/Zahran Unpad/Skripsi Analisis Sentimen/Code/Website/web/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8903dcf0377865c7/Dokumen/Punya Zahran/Zahran Unpad/Skripsi Analisis Sentimen/Code/Website - Copy/web/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{02D57D6A-D35C-6846-BB4C-8A6B74773428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{744AA726-BA6E-44CB-B273-767C262993B5}"/>
@@ -8862,8 +8862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2895" workbookViewId="0">
-      <selection sqref="A1:B2919"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>